<commit_message>
Pruebas hasta test.convenios nada de onjetsConvenio
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
+++ b/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="4140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="5070"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>01</t>
   </si>
@@ -221,15 +221,6 @@
     <t>7342534</t>
   </si>
   <si>
-    <t>7342535</t>
-  </si>
-  <si>
-    <t>7342536</t>
-  </si>
-  <si>
-    <t>7342537</t>
-  </si>
-  <si>
     <t>7342538</t>
   </si>
   <si>
@@ -243,6 +234,42 @@
   </si>
   <si>
     <t>davivienda.com.co</t>
+  </si>
+  <si>
+    <t>tigoUne</t>
+  </si>
+  <si>
+    <t>www.tigo.com.co</t>
+  </si>
+  <si>
+    <t>recaudos@tigoune.com.co</t>
+  </si>
+  <si>
+    <t>carrera 30n #12-2</t>
+  </si>
+  <si>
+    <t>Movistar</t>
+  </si>
+  <si>
+    <t>www.movistar.com</t>
+  </si>
+  <si>
+    <t>recaudos@movistar.com</t>
+  </si>
+  <si>
+    <t>carrera 45n #12-2</t>
+  </si>
+  <si>
+    <t>Edeq</t>
+  </si>
+  <si>
+    <t>www.edeq.com.co</t>
+  </si>
+  <si>
+    <t>recaudos@edeq.com.co</t>
+  </si>
+  <si>
+    <t>carrera 13 # 15 -16</t>
   </si>
 </sst>
 </file>
@@ -610,15 +637,13 @@
   <dimension ref="A2:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -679,13 +704,13 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -704,20 +729,29 @@
       </c>
       <c r="J3" t="s">
         <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>61</v>
+      <c r="B4" s="4">
+        <v>7552233</v>
+      </c>
+      <c r="C4" s="4">
+        <v>7552266</v>
+      </c>
+      <c r="D4" s="4">
+        <v>7489630</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>62</v>
@@ -738,25 +772,25 @@
         <v>67</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -764,13 +798,13 @@
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
@@ -786,6 +820,15 @@
       </c>
       <c r="J5" t="s">
         <v>31</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -793,13 +836,13 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>32</v>
@@ -845,14 +888,14 @@
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>52</v>
+      <c r="B7" s="4">
+        <v>3109885641</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3128321669</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3154079988</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>53</v>
@@ -871,6 +914,15 @@
       </c>
       <c r="J7" s="4" t="s">
         <v>58</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -878,13 +930,13 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -903,6 +955,15 @@
       </c>
       <c r="J8" t="s">
         <v>49</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -910,13 +971,13 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
@@ -935,15 +996,30 @@
       </c>
       <c r="J9" t="s">
         <v>49</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="C6:Q6" r:id="rId3" display="pagos@Efectivo.com"/>
+    <hyperlink ref="K5" r:id="rId1"/>
+    <hyperlink ref="E6:Q6" r:id="rId2" display="pagos@Efectivo.com"/>
+    <hyperlink ref="K6" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="D6" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="B6" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pruebas hasta conbenio de recaudos full
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
+++ b/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>01</t>
   </si>
@@ -270,6 +270,24 @@
   </si>
   <si>
     <t>carrera 13 # 15 -16</t>
+  </si>
+  <si>
+    <t>7558829</t>
+  </si>
+  <si>
+    <t>75398</t>
+  </si>
+  <si>
+    <t>3698547</t>
+  </si>
+  <si>
+    <t>3108228425</t>
+  </si>
+  <si>
+    <t>3121715639</t>
+  </si>
+  <si>
+    <t>312321666</t>
   </si>
 </sst>
 </file>
@@ -637,7 +655,7 @@
   <dimension ref="A2:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,14 +762,14 @@
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="4">
-        <v>7552233</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7552266</v>
-      </c>
-      <c r="D4" s="4">
-        <v>7489630</v>
+      <c r="B4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>62</v>
@@ -888,14 +906,14 @@
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4">
-        <v>3109885641</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3128321669</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3154079988</v>
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
pruebas hasta convenio de recaudos full
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
+++ b/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>01</t>
   </si>
@@ -270,6 +270,24 @@
   </si>
   <si>
     <t>carrera 13 # 15 -16</t>
+  </si>
+  <si>
+    <t>7558829</t>
+  </si>
+  <si>
+    <t>75398</t>
+  </si>
+  <si>
+    <t>3698547</t>
+  </si>
+  <si>
+    <t>3108228425</t>
+  </si>
+  <si>
+    <t>3121715639</t>
+  </si>
+  <si>
+    <t>312321666</t>
   </si>
 </sst>
 </file>
@@ -637,7 +655,7 @@
   <dimension ref="A2:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,14 +762,14 @@
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="4">
-        <v>7552233</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7552266</v>
-      </c>
-      <c r="D4" s="4">
-        <v>7489630</v>
+      <c r="B4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>62</v>
@@ -888,14 +906,14 @@
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4">
-        <v>3109885641</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3128321669</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3154079988</v>
+      <c r="B7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Varios cambion sin mucha importancia
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
+++ b/MercuryTours/Resources/datapool/clientesRecaudos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>01</t>
   </si>
@@ -224,9 +224,6 @@
     <t>7342538</t>
   </si>
   <si>
-    <t>7342539</t>
-  </si>
-  <si>
     <t>7342540</t>
   </si>
   <si>
@@ -287,7 +284,22 @@
     <t>3121715639</t>
   </si>
   <si>
-    <t>312321666</t>
+    <t>recaudos@algo.com</t>
+  </si>
+  <si>
+    <t>Efigas</t>
+  </si>
+  <si>
+    <t>www.efigas.com.co</t>
+  </si>
+  <si>
+    <t>recaudoster@efigas.com</t>
+  </si>
+  <si>
+    <t>carrera 14 #12n-9</t>
+  </si>
+  <si>
+    <t>3123216661</t>
   </si>
 </sst>
 </file>
@@ -655,7 +667,7 @@
   <dimension ref="A2:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,16 +734,16 @@
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -756,6 +768,9 @@
       </c>
       <c r="M3" t="s">
         <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -763,16 +778,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>62</v>
+      <c r="E4">
+        <v>4526988</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>63</v>
@@ -802,13 +817,13 @@
         <v>68</v>
       </c>
       <c r="O4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -816,16 +831,16 @@
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
+        <v>77</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -846,7 +861,10 @@
         <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -854,16 +872,16 @@
         <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>32</v>
@@ -893,7 +911,7 @@
         <v>32</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>32</v>
@@ -907,16 +925,16 @@
         <v>38</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>94</v>
+      </c>
+      <c r="E7">
+        <v>3108226932</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>54</v>
@@ -941,6 +959,9 @@
       </c>
       <c r="M7" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -948,16 +969,16 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
@@ -982,6 +1003,9 @@
       </c>
       <c r="M8" t="s">
         <v>43</v>
+      </c>
+      <c r="O8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -989,16 +1013,16 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
         <v>45</v>
@@ -1023,21 +1047,26 @@
       </c>
       <c r="M9" t="s">
         <v>43</v>
+      </c>
+      <c r="O9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K5" r:id="rId1"/>
-    <hyperlink ref="E6:Q6" r:id="rId2" display="pagos@Efectivo.com"/>
-    <hyperlink ref="K6" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="D6" r:id="rId7"/>
-    <hyperlink ref="B5" r:id="rId8"/>
-    <hyperlink ref="B6" r:id="rId9"/>
+    <hyperlink ref="K6" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="B5" r:id="rId7"/>
+    <hyperlink ref="B6" r:id="rId8"/>
+    <hyperlink ref="O6" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId10"/>
+    <hyperlink ref="E6" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>